<commit_message>
루시 찌르기, 가르기 스킬 AiData Atk_Type 을 Select Emeny 로 수정
</commit_message>
<xml_diff>
--- a/Assets/ERang/Excels/AiData.xlsx
+++ b/Assets/ERang/Excels/AiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shpapa\Desktop\repo2\repo\Assets\ERang\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repo\Assets\ERang\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4720056A-1911-43BA-821D-8D663C536C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC307B94-3955-4DED-89C7-DFBFE2DAFEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5440" yWindow="1380" windowWidth="31950" windowHeight="17430" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="77">
   <si>
     <t>#NameDesc</t>
   </si>
@@ -265,6 +265,10 @@
   </si>
   <si>
     <t>81002000, 81002001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select Enemy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -740,27 +744,27 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="8.75" style="1"/>
     <col min="2" max="2" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.75" style="1"/>
-    <col min="4" max="4" width="22.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.58203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.75" style="1"/>
-    <col min="8" max="8" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.75" style="1"/>
-    <col min="10" max="10" width="16.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5">
+    <row r="1" spans="1:11" ht="17">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -795,7 +799,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5">
+    <row r="2" spans="1:11" ht="17">
       <c r="A2" s="4">
         <v>1001</v>
       </c>
@@ -826,7 +830,7 @@
         <v>70001</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.5">
+    <row r="3" spans="1:11" ht="17">
       <c r="A3" s="4">
         <v>1002</v>
       </c>
@@ -859,7 +863,7 @@
         <v>70002</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16.5">
+    <row r="4" spans="1:11" ht="17">
       <c r="A4" s="4">
         <v>1003</v>
       </c>
@@ -890,7 +894,7 @@
         <v>70003</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5">
+    <row r="5" spans="1:11" ht="17">
       <c r="A5" s="4">
         <v>1004</v>
       </c>
@@ -921,7 +925,7 @@
         <v>70004</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16.5">
+    <row r="6" spans="1:11" ht="17">
       <c r="A6" s="4">
         <v>1005</v>
       </c>
@@ -954,7 +958,7 @@
         <v>70005</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16.5">
+    <row r="7" spans="1:11" ht="17">
       <c r="A7" s="4">
         <v>1006</v>
       </c>
@@ -985,7 +989,7 @@
         <v>70006</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5">
+    <row r="8" spans="1:11" ht="17">
       <c r="A8" s="4">
         <v>1007</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>70007</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16.5">
+    <row r="9" spans="1:11" ht="17">
       <c r="A9" s="4">
         <v>1008</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>70008</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5">
+    <row r="10" spans="1:11" ht="17">
       <c r="A10" s="4">
         <v>1009</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>70009</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16.5">
+    <row r="11" spans="1:11" ht="17">
       <c r="A11" s="4">
         <v>1010</v>
       </c>
@@ -1092,7 +1096,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1109,7 +1113,7 @@
         <v>70010</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5">
+    <row r="12" spans="1:11" ht="17">
       <c r="A12" s="4">
         <v>1011</v>
       </c>
@@ -1140,7 +1144,7 @@
         <v>70011</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16.5">
+    <row r="13" spans="1:11" ht="17">
       <c r="A13" s="4">
         <v>1012</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>70012</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5">
+    <row r="14" spans="1:11" ht="17">
       <c r="A14" s="4">
         <v>1013</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>70013</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16.5">
+    <row r="15" spans="1:11" ht="17">
       <c r="A15" s="4">
         <v>1014</v>
       </c>
@@ -1227,7 +1231,7 @@
         <v>70014</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16.5">
+    <row r="16" spans="1:11" ht="17">
       <c r="A16" s="4">
         <v>2001</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>70015</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16.5">
+    <row r="17" spans="1:11" ht="17">
       <c r="A17" s="4">
         <v>2002</v>
       </c>
@@ -1289,7 +1293,7 @@
         <v>70016</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16.5">
+    <row r="18" spans="1:11" ht="17">
       <c r="A18" s="4">
         <v>2003</v>
       </c>
@@ -1316,7 +1320,7 @@
         <v>70017</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16.5">
+    <row r="19" spans="1:11" ht="17">
       <c r="A19" s="4">
         <v>2004</v>
       </c>
@@ -1343,7 +1347,7 @@
         <v>70018</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16.5">
+    <row r="20" spans="1:11" ht="17">
       <c r="A20" s="4">
         <v>3001</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>70019</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16.5">
+    <row r="21" spans="1:11" ht="17">
       <c r="A21" s="4">
         <v>3002</v>
       </c>
@@ -1405,7 +1409,7 @@
         <v>70020</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16.5">
+    <row r="22" spans="1:11" ht="17">
       <c r="A22" s="4">
         <v>3003</v>
       </c>
@@ -1436,7 +1440,7 @@
         <v>70021</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16.5">
+    <row r="23" spans="1:11" ht="17">
       <c r="A23" s="4">
         <v>4001</v>
       </c>
@@ -1467,7 +1471,7 @@
         <v>70022</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16.5">
+    <row r="24" spans="1:11" ht="17">
       <c r="A24" s="4">
         <v>4002</v>
       </c>
@@ -1498,7 +1502,7 @@
         <v>70023</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16.5">
+    <row r="25" spans="1:11" ht="17">
       <c r="A25" s="4">
         <v>4003</v>
       </c>
@@ -1529,7 +1533,7 @@
         <v>70024</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16.5">
+    <row r="26" spans="1:11" ht="17">
       <c r="A26" s="4">
         <v>4004</v>
       </c>
@@ -1558,7 +1562,7 @@
         <v>70025</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16.5">
+    <row r="27" spans="1:11" ht="17">
       <c r="A27" s="4">
         <v>90001</v>
       </c>
@@ -1589,7 +1593,7 @@
         <v>90001</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16.5">
+    <row r="28" spans="1:11" ht="17">
       <c r="A28" s="4">
         <v>90002</v>
       </c>
@@ -1620,7 +1624,7 @@
         <v>90002</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="16.5">
+    <row r="29" spans="1:11" ht="17">
       <c r="A29" s="4">
         <v>90003</v>
       </c>
@@ -1647,7 +1651,7 @@
         <v>90003</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="16.5">
+    <row r="30" spans="1:11" ht="17">
       <c r="A30" s="4">
         <v>90004</v>
       </c>
@@ -1674,7 +1678,7 @@
         <v>90004</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="16.5">
+    <row r="31" spans="1:11" ht="17">
       <c r="A31" s="4">
         <v>90005</v>
       </c>
@@ -1701,7 +1705,7 @@
         <v>90005</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16.5">
+    <row r="32" spans="1:11" ht="17">
       <c r="A32" s="4">
         <v>90006</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16.5">
+    <row r="33" spans="1:11" ht="17">
       <c r="A33" s="4">
         <v>100001</v>
       </c>
@@ -1755,7 +1759,7 @@
         <v>100001</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="16.5">
+    <row r="34" spans="1:11" ht="17">
       <c r="A34" s="4">
         <v>100002</v>
       </c>
@@ -1782,7 +1786,7 @@
         <v>100002</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="16.5">
+    <row r="35" spans="1:11" ht="17">
       <c r="A35" s="4">
         <v>100011</v>
       </c>
@@ -1809,7 +1813,7 @@
         <v>100011</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="16.5">
+    <row r="36" spans="1:11" ht="17">
       <c r="A36" s="4">
         <v>100012</v>
       </c>
@@ -1836,7 +1840,7 @@
         <v>100012</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="16.5">
+    <row r="37" spans="1:11" ht="17">
       <c r="A37" s="4">
         <v>100013</v>
       </c>
@@ -1863,7 +1867,7 @@
         <v>100013</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16.5">
+    <row r="38" spans="1:11" ht="17">
       <c r="A38" s="7">
         <v>100014</v>
       </c>
@@ -1890,7 +1894,7 @@
         <v>100026</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="16.5">
+    <row r="39" spans="1:11" ht="17">
       <c r="A39" s="4">
         <v>8100100</v>
       </c>
@@ -1904,7 +1908,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>15</v>
@@ -1921,7 +1925,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16.5">
+    <row r="40" spans="1:11" ht="17">
       <c r="A40" s="4">
         <v>8100200</v>
       </c>
@@ -1935,7 +1939,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="F40" s="4">
         <v>1</v>

</xml_diff>